<commit_message>
update sprint02 - pós entrega
</commit_message>
<xml_diff>
--- a/Docs/Passagem das Frentes/Rotação.xlsx
+++ b/Docs/Passagem das Frentes/Rotação.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6963eeb36638e18/Documentos/Sptech/projeto-sprint-2/queijo-minas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Área de Trabalho\Backup SPTech\queijo-minas\Docs\Passagem das Frentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{563C90C5-758B-4058-8A5B-26CD2DCC7082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F16220A-1F2C-4A37-8C03-9C1756205799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10741566-B90A-4738-BBBA-70BFDD454DC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{10741566-B90A-4738-BBBA-70BFDD454DC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -914,7 +914,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1101,6 +1101,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9fdc8751-6fef-42ec-b05c-835dd8c535b4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD11765F9AC0004AAF0A4CAAFDFAF16A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fcbceef0f5a4544440e3d6b2cafd9188">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9fdc8751-6fef-42ec-b05c-835dd8c535b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e373b3d822a661c9833b36363258e1fe" ns3:_="">
     <xsd:import namespace="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
@@ -1256,24 +1273,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98DB6198-34CA-4A38-B6FC-514D22CAEC94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9fdc8751-6fef-42ec-b05c-835dd8c535b4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA7C07F-7232-46B3-93CE-9F5B1C78672C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D85E1064-EADB-4F15-86F6-E9EBE4B2AF19}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1289,22 +1307,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA7C07F-7232-46B3-93CE-9F5B1C78672C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98DB6198-34CA-4A38-B6FC-514D22CAEC94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>